<commit_message>
- Filesystem is set to Read Write if not connected to USB - Fixed bug when no config.txt file exists and attempting to write to config.txt - Added regions to set limits on frequency, power, and check for invalid profiles - Updated screens.html to reflect UI changes - Fixed bug with volume and brightness changes not saving to config.txt
</commit_message>
<xml_diff>
--- a/Documentation/Tasks.xlsx
+++ b/Documentation/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Armachat\Armachat-circuitpython\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3634FE8D-F6C4-45BF-8C8A-C2607C840C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A556E9-4CC0-4BED-B472-FF84E742E5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{48331F84-D6AF-4212-9807-071E67B15285}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{48331F84-D6AF-4212-9807-071E67B15285}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="184">
   <si>
     <t>Screen</t>
   </si>
@@ -582,15 +582,25 @@
   </si>
   <si>
     <t>Module</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>module</t>
+  </si>
+  <si>
+    <t>Array</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -696,7 +706,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -737,6 +747,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -745,6 +758,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1075,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C985E-F91F-471A-B04D-0671E5EAB4DD}">
   <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
@@ -2374,30 +2392,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="20"/>
+      <c r="C1" s="21"/>
       <c r="D1">
         <f>COUNTA(A6:A501)</f>
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="21"/>
       <c r="D2">
         <f>D1-COUNTIF(D6:D501,TRUE)</f>
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="20"/>
+      <c r="C3" s="21"/>
       <c r="D3" s="9">
         <f>(D1-D2)/D1</f>
         <v>0.77777777777777779</v>
@@ -2870,12 +2888,12 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -2952,12 +2970,12 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -3237,28 +3255,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="22"/>
+      <c r="B1" s="23"/>
       <c r="C1" s="4">
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="B2" s="22"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="4">
         <v>902</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>176</v>
       </c>
-      <c r="B3" s="22"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="4">
         <v>928</v>
       </c>
@@ -7894,25 +7912,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0905176-8170-4141-BFF8-73C1F588C34D}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="82" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -8392,7 +8411,7 @@
         <v>922.5</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>172</v>
       </c>
@@ -8427,7 +8446,512 @@
         <v>915</v>
       </c>
     </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="I20" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B21" s="7">
+        <v>915</v>
+      </c>
+      <c r="C21" s="24">
+        <v>915</v>
+      </c>
+      <c r="D21" s="25">
+        <v>902</v>
+      </c>
+      <c r="E21" s="25">
+        <v>928</v>
+      </c>
+      <c r="F21" s="4">
+        <v>100</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="4">
+        <v>30</v>
+      </c>
+      <c r="I21" s="26" t="str">
+        <f>"{""" &amp;$A$20 &amp; """: """ &amp; A21 &amp; """, """  &amp; $C$20 &amp; """: " &amp; C21 &amp; ", """ &amp; $D$20 &amp; """: " &amp;D21 &amp; ", """ &amp; $E$20 &amp; """: " &amp; E21 &amp; ", """ &amp; $F$20 &amp; """: " &amp; F21 &amp; ", """ &amp; $G$20 &amp; """: " &amp; G21 &amp; ", """ &amp; $H$20 &amp; """: " &amp; H21 &amp; "},"</f>
+        <v>{"region": "US", "freqCenter": 915, "freqStart": 902, "freqEnd": 928, "dutyCycle": 100, "spacing": 0, "powerLimit": 30},</v>
+      </c>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+    </row>
+    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B22" s="7">
+        <v>433</v>
+      </c>
+      <c r="C22" s="24">
+        <v>433.5</v>
+      </c>
+      <c r="D22" s="25">
+        <v>433</v>
+      </c>
+      <c r="E22" s="25">
+        <v>434</v>
+      </c>
+      <c r="F22" s="4">
+        <v>10</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0</v>
+      </c>
+      <c r="H22" s="4">
+        <v>12</v>
+      </c>
+      <c r="I22" s="26" t="str">
+        <f t="shared" ref="I22:I33" si="2">"{""" &amp;$A$20 &amp; """: """ &amp; A22 &amp; """, """  &amp; $C$20 &amp; """: " &amp; C22 &amp; ", """ &amp; $D$20 &amp; """: " &amp;D22 &amp; ", """ &amp; $E$20 &amp; """: " &amp; E22 &amp; ", """ &amp; $F$20 &amp; """: " &amp; F22 &amp; ", """ &amp; $G$20 &amp; """: " &amp; G22 &amp; ", """ &amp; $H$20 &amp; """: " &amp; H22 &amp; "},"</f>
+        <v>{"region": "EU433", "freqCenter": 433.5, "freqStart": 433, "freqEnd": 434, "dutyCycle": 10, "spacing": 0, "powerLimit": 12},</v>
+      </c>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+    </row>
+    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23" s="7">
+        <v>868</v>
+      </c>
+      <c r="C23" s="24">
+        <v>869.52499999999998</v>
+      </c>
+      <c r="D23" s="25">
+        <v>869.4</v>
+      </c>
+      <c r="E23" s="25">
+        <v>869.65</v>
+      </c>
+      <c r="F23" s="4">
+        <v>10</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+      <c r="H23" s="4">
+        <v>16</v>
+      </c>
+      <c r="I23" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>{"region": "EU868", "freqCenter": 869.525, "freqStart": 869.4, "freqEnd": 869.65, "dutyCycle": 10, "spacing": 0, "powerLimit": 16},</v>
+      </c>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
+    </row>
+    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B24" s="7">
+        <v>433</v>
+      </c>
+      <c r="C24" s="24">
+        <v>490</v>
+      </c>
+      <c r="D24" s="25">
+        <v>470</v>
+      </c>
+      <c r="E24" s="25">
+        <v>510</v>
+      </c>
+      <c r="F24" s="4">
+        <v>100</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0</v>
+      </c>
+      <c r="H24" s="4">
+        <v>19</v>
+      </c>
+      <c r="I24" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>{"region": "CN", "freqCenter": 490, "freqStart": 470, "freqEnd": 510, "dutyCycle": 100, "spacing": 0, "powerLimit": 19},</v>
+      </c>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+    </row>
+    <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B25" s="7">
+        <v>915</v>
+      </c>
+      <c r="C25" s="24">
+        <v>924.3</v>
+      </c>
+      <c r="D25" s="25">
+        <v>920.8</v>
+      </c>
+      <c r="E25" s="25">
+        <v>927.8</v>
+      </c>
+      <c r="F25" s="4">
+        <v>100</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
+      <c r="H25" s="4">
+        <v>16</v>
+      </c>
+      <c r="I25" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>{"region": "JP", "freqCenter": 924.3, "freqStart": 920.8, "freqEnd": 927.8, "dutyCycle": 100, "spacing": 0, "powerLimit": 16},</v>
+      </c>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="26"/>
+    </row>
+    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" s="7">
+        <v>915</v>
+      </c>
+      <c r="C26" s="24">
+        <v>921.5</v>
+      </c>
+      <c r="D26" s="25">
+        <v>915</v>
+      </c>
+      <c r="E26" s="25">
+        <v>928</v>
+      </c>
+      <c r="F26" s="4">
+        <v>100</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0</v>
+      </c>
+      <c r="H26" s="4">
+        <v>30</v>
+      </c>
+      <c r="I26" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>{"region": "ANZ", "freqCenter": 921.5, "freqStart": 915, "freqEnd": 928, "dutyCycle": 100, "spacing": 0, "powerLimit": 30},</v>
+      </c>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
+    </row>
+    <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B27" s="7">
+        <v>868</v>
+      </c>
+      <c r="C27" s="24">
+        <v>868.95</v>
+      </c>
+      <c r="D27" s="25">
+        <v>868.7</v>
+      </c>
+      <c r="E27" s="25">
+        <v>869.2</v>
+      </c>
+      <c r="F27" s="4">
+        <v>100</v>
+      </c>
+      <c r="G27" s="4">
+        <v>0</v>
+      </c>
+      <c r="H27" s="4">
+        <v>20</v>
+      </c>
+      <c r="I27" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>{"region": "RU", "freqCenter": 868.95, "freqStart": 868.7, "freqEnd": 869.2, "dutyCycle": 100, "spacing": 0, "powerLimit": 20},</v>
+      </c>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="26"/>
+    </row>
+    <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B28" s="7">
+        <v>915</v>
+      </c>
+      <c r="C28" s="24">
+        <v>921.5</v>
+      </c>
+      <c r="D28" s="25">
+        <v>920</v>
+      </c>
+      <c r="E28" s="25">
+        <v>923</v>
+      </c>
+      <c r="F28" s="4">
+        <v>100</v>
+      </c>
+      <c r="G28" s="4">
+        <v>0</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0</v>
+      </c>
+      <c r="I28" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>{"region": "KR", "freqCenter": 921.5, "freqStart": 920, "freqEnd": 923, "dutyCycle": 100, "spacing": 0, "powerLimit": 0},</v>
+      </c>
+      <c r="J28" s="26"/>
+      <c r="K28" s="26"/>
+      <c r="L28" s="26"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="26"/>
+    </row>
+    <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29" s="7">
+        <v>915</v>
+      </c>
+      <c r="C29" s="24">
+        <v>922.5</v>
+      </c>
+      <c r="D29" s="25">
+        <v>920</v>
+      </c>
+      <c r="E29" s="25">
+        <v>925</v>
+      </c>
+      <c r="F29" s="4">
+        <v>100</v>
+      </c>
+      <c r="G29" s="4">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0</v>
+      </c>
+      <c r="I29" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>{"region": "TW", "freqCenter": 922.5, "freqStart": 920, "freqEnd": 925, "dutyCycle": 100, "spacing": 0, "powerLimit": 0},</v>
+      </c>
+      <c r="J29" s="26"/>
+      <c r="K29" s="26"/>
+      <c r="L29" s="26"/>
+      <c r="M29" s="26"/>
+      <c r="N29" s="26"/>
+    </row>
+    <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B30" s="7">
+        <v>866</v>
+      </c>
+      <c r="C30" s="24">
+        <v>866</v>
+      </c>
+      <c r="D30" s="25">
+        <v>865</v>
+      </c>
+      <c r="E30" s="25">
+        <v>867</v>
+      </c>
+      <c r="F30" s="4">
+        <v>100</v>
+      </c>
+      <c r="G30" s="4">
+        <v>0</v>
+      </c>
+      <c r="H30" s="4">
+        <v>30</v>
+      </c>
+      <c r="I30" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>{"region": "IN", "freqCenter": 866, "freqStart": 865, "freqEnd": 867, "dutyCycle": 100, "spacing": 0, "powerLimit": 30},</v>
+      </c>
+      <c r="J30" s="26"/>
+      <c r="K30" s="26"/>
+      <c r="L30" s="26"/>
+      <c r="M30" s="26"/>
+      <c r="N30" s="26"/>
+    </row>
+    <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B31" s="7">
+        <v>866</v>
+      </c>
+      <c r="C31" s="24">
+        <v>866</v>
+      </c>
+      <c r="D31" s="25">
+        <v>864</v>
+      </c>
+      <c r="E31" s="25">
+        <v>868</v>
+      </c>
+      <c r="F31" s="4">
+        <v>100</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0</v>
+      </c>
+      <c r="I31" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>{"region": "NZ865", "freqCenter": 866, "freqStart": 864, "freqEnd": 868, "dutyCycle": 100, "spacing": 0, "powerLimit": 0},</v>
+      </c>
+      <c r="J31" s="26"/>
+      <c r="K31" s="26"/>
+      <c r="L31" s="26"/>
+      <c r="M31" s="26"/>
+      <c r="N31" s="26"/>
+    </row>
+    <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B32" s="7">
+        <v>915</v>
+      </c>
+      <c r="C32" s="24">
+        <v>922.5</v>
+      </c>
+      <c r="D32" s="25">
+        <v>920</v>
+      </c>
+      <c r="E32" s="25">
+        <v>925</v>
+      </c>
+      <c r="F32" s="4">
+        <v>100</v>
+      </c>
+      <c r="G32" s="4">
+        <v>0</v>
+      </c>
+      <c r="H32" s="4">
+        <v>16</v>
+      </c>
+      <c r="I32" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>{"region": "TH", "freqCenter": 922.5, "freqStart": 920, "freqEnd": 925, "dutyCycle": 100, "spacing": 0, "powerLimit": 16},</v>
+      </c>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+      <c r="L32" s="26"/>
+      <c r="M32" s="26"/>
+      <c r="N32" s="26"/>
+    </row>
+    <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B33" s="7">
+        <v>915</v>
+      </c>
+      <c r="C33" s="24">
+        <v>915</v>
+      </c>
+      <c r="D33" s="25">
+        <v>902</v>
+      </c>
+      <c r="E33" s="25">
+        <v>928</v>
+      </c>
+      <c r="F33" s="4">
+        <v>100</v>
+      </c>
+      <c r="G33" s="4">
+        <v>0</v>
+      </c>
+      <c r="H33" s="4">
+        <v>30</v>
+      </c>
+      <c r="I33" s="26" t="str">
+        <f t="shared" si="2"/>
+        <v>{"region": "Unset", "freqCenter": 915, "freqStart": 902, "freqEnd": 928, "dutyCycle": 100, "spacing": 0, "powerLimit": 30},</v>
+      </c>
+      <c r="J33" s="26"/>
+      <c r="K33" s="26"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="26"/>
+      <c r="N33" s="26"/>
+    </row>
   </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="I32:N32"/>
+    <mergeCell ref="I33:N33"/>
+    <mergeCell ref="I26:N26"/>
+    <mergeCell ref="I27:N27"/>
+    <mergeCell ref="I28:N28"/>
+    <mergeCell ref="I29:N29"/>
+    <mergeCell ref="I30:N30"/>
+    <mergeCell ref="I31:N31"/>
+    <mergeCell ref="I20:N20"/>
+    <mergeCell ref="I21:N21"/>
+    <mergeCell ref="I22:N22"/>
+    <mergeCell ref="I23:N23"/>
+    <mergeCell ref="I24:N24"/>
+    <mergeCell ref="I25:N25"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented change of region in setup-radio screen
</commit_message>
<xml_diff>
--- a/Documentation/Tasks.xlsx
+++ b/Documentation/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Armachat\Armachat-circuitpython\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E009C190-854C-4AA8-B191-F23D1848AB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538E2677-64B3-411D-A0B9-1E26355D2D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{48331F84-D6AF-4212-9807-071E67B15285}"/>
   </bookViews>
@@ -1117,7 +1117,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
+      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,7 +1142,7 @@
       </c>
       <c r="D2">
         <f>D1-COUNTIF(D6:D502,TRUE)</f>
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1151,7 +1151,7 @@
       </c>
       <c r="D3" s="9">
         <f>(D1-D2)/D1</f>
-        <v>0.74725274725274726</v>
+        <v>0.75824175824175821</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1810,7 +1810,9 @@
       <c r="C53" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="D53" s="4"/>
+      <c r="D53" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
@@ -8965,12 +8967,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="I25:N25"/>
-    <mergeCell ref="I20:N20"/>
-    <mergeCell ref="I21:N21"/>
-    <mergeCell ref="I22:N22"/>
-    <mergeCell ref="I23:N23"/>
-    <mergeCell ref="I24:N24"/>
     <mergeCell ref="I32:N32"/>
     <mergeCell ref="I33:N33"/>
     <mergeCell ref="I26:N26"/>
@@ -8979,6 +8975,12 @@
     <mergeCell ref="I29:N29"/>
     <mergeCell ref="I30:N30"/>
     <mergeCell ref="I31:N31"/>
+    <mergeCell ref="I25:N25"/>
+    <mergeCell ref="I20:N20"/>
+    <mergeCell ref="I21:N21"/>
+    <mergeCell ref="I22:N22"/>
+    <mergeCell ref="I23:N23"/>
+    <mergeCell ref="I24:N24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>

<commit_message>
Modified the region edit to select next profile that has a valid bandwidth for the region
</commit_message>
<xml_diff>
--- a/Documentation/Tasks.xlsx
+++ b/Documentation/Tasks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Armachat\Armachat-circuitpython\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Armachat-circuitpython\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538E2677-64B3-411D-A0B9-1E26355D2D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD72D78-3CA0-4DBF-8729-0197B1638A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{48331F84-D6AF-4212-9807-071E67B15285}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="4" xr2:uid="{48331F84-D6AF-4212-9807-071E67B15285}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="191">
   <si>
     <t>Screen</t>
   </si>
@@ -607,6 +607,12 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>bw (KHz)</t>
+  </si>
+  <si>
+    <t>bw (MHz)</t>
   </si>
 </sst>
 </file>
@@ -722,7 +728,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -774,6 +780,9 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -786,6 +795,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1115,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C985E-F91F-471A-B04D-0671E5EAB4DD}">
   <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
@@ -2422,30 +2435,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="25"/>
+      <c r="C1" s="26"/>
       <c r="D1">
         <f>COUNTA(A6:A501)</f>
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="25"/>
+      <c r="C2" s="26"/>
       <c r="D2">
         <f>D1-COUNTIF(D6:D501,TRUE)</f>
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="25"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="9">
         <f>(D1-D2)/D1</f>
         <v>0.77777777777777779</v>
@@ -2918,12 +2931,12 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -3000,12 +3013,12 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -3285,28 +3298,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="B2" s="27"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="4">
         <v>902</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="B3" s="27"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="4">
         <v>928</v>
       </c>
@@ -7942,19 +7955,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0905176-8170-4141-BFF8-73C1F588C34D}">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -8501,14 +8514,14 @@
       <c r="H20" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="I20" s="26" t="s">
+      <c r="I20" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
@@ -8535,15 +8548,15 @@
       <c r="H21" s="4">
         <v>30</v>
       </c>
-      <c r="I21" s="28" t="str">
+      <c r="I21" s="29" t="str">
         <f>"{""" &amp;$A$20 &amp; """: """ &amp; A21 &amp; """, """  &amp; $C$20 &amp; """: " &amp; C21 &amp; ", """ &amp; $D$20 &amp; """: " &amp;D21 &amp; ", """ &amp; $E$20 &amp; """: " &amp; E21 &amp; ", """ &amp; $F$20 &amp; """: " &amp; F21 &amp; ", """ &amp; $G$20 &amp; """: " &amp; G21 &amp; ", """ &amp; $H$20 &amp; """: " &amp; H21 &amp; "},"</f>
         <v>{"region": "US", "freqCenter": 915, "freqStart": 902, "freqEnd": 928, "dutyCycle": 100, "spacing": 0, "powerLimit": 30},</v>
       </c>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
@@ -8570,15 +8583,15 @@
       <c r="H22" s="4">
         <v>12</v>
       </c>
-      <c r="I22" s="28" t="str">
+      <c r="I22" s="29" t="str">
         <f t="shared" ref="I22:I33" si="2">"{""" &amp;$A$20 &amp; """: """ &amp; A22 &amp; """, """  &amp; $C$20 &amp; """: " &amp; C22 &amp; ", """ &amp; $D$20 &amp; """: " &amp;D22 &amp; ", """ &amp; $E$20 &amp; """: " &amp; E22 &amp; ", """ &amp; $F$20 &amp; """: " &amp; F22 &amp; ", """ &amp; $G$20 &amp; """: " &amp; G22 &amp; ", """ &amp; $H$20 &amp; """: " &amp; H22 &amp; "},"</f>
         <v>{"region": "EU433", "freqCenter": 433.5, "freqStart": 433, "freqEnd": 434, "dutyCycle": 10, "spacing": 0, "powerLimit": 12},</v>
       </c>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
     </row>
     <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
@@ -8605,15 +8618,15 @@
       <c r="H23" s="4">
         <v>16</v>
       </c>
-      <c r="I23" s="28" t="str">
+      <c r="I23" s="29" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "EU868", "freqCenter": 869.525, "freqStart": 869.4, "freqEnd": 869.65, "dutyCycle": 10, "spacing": 0, "powerLimit": 16},</v>
       </c>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
     </row>
     <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -8640,15 +8653,15 @@
       <c r="H24" s="4">
         <v>19</v>
       </c>
-      <c r="I24" s="28" t="str">
+      <c r="I24" s="29" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "CN", "freqCenter": 490, "freqStart": 470, "freqEnd": 510, "dutyCycle": 100, "spacing": 0, "powerLimit": 19},</v>
       </c>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
-      <c r="N24" s="28"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
     </row>
     <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -8675,15 +8688,15 @@
       <c r="H25" s="4">
         <v>16</v>
       </c>
-      <c r="I25" s="28" t="str">
+      <c r="I25" s="29" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "JP", "freqCenter": 924.3, "freqStart": 920.8, "freqEnd": 927.8, "dutyCycle": 100, "spacing": 0, "powerLimit": 16},</v>
       </c>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="28"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
     </row>
     <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -8710,15 +8723,15 @@
       <c r="H26" s="4">
         <v>30</v>
       </c>
-      <c r="I26" s="28" t="str">
+      <c r="I26" s="29" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "ANZ", "freqCenter": 921.5, "freqStart": 915, "freqEnd": 928, "dutyCycle": 100, "spacing": 0, "powerLimit": 30},</v>
       </c>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
     </row>
     <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -8745,15 +8758,15 @@
       <c r="H27" s="4">
         <v>20</v>
       </c>
-      <c r="I27" s="28" t="str">
+      <c r="I27" s="29" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "RU", "freqCenter": 868.95, "freqStart": 868.7, "freqEnd": 869.2, "dutyCycle": 100, "spacing": 0, "powerLimit": 20},</v>
       </c>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="28"/>
-      <c r="N27" s="28"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
     </row>
     <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
@@ -8780,15 +8793,15 @@
       <c r="H28" s="4">
         <v>0</v>
       </c>
-      <c r="I28" s="28" t="str">
+      <c r="I28" s="29" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "KR", "freqCenter": 921.5, "freqStart": 920, "freqEnd": 923, "dutyCycle": 100, "spacing": 0, "powerLimit": 0},</v>
       </c>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
-      <c r="N28" s="28"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
     </row>
     <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
@@ -8815,15 +8828,15 @@
       <c r="H29" s="4">
         <v>0</v>
       </c>
-      <c r="I29" s="28" t="str">
+      <c r="I29" s="29" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "TW", "freqCenter": 922.5, "freqStart": 920, "freqEnd": 925, "dutyCycle": 100, "spacing": 0, "powerLimit": 0},</v>
       </c>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
     </row>
     <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
@@ -8850,15 +8863,15 @@
       <c r="H30" s="4">
         <v>30</v>
       </c>
-      <c r="I30" s="28" t="str">
+      <c r="I30" s="29" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "IN", "freqCenter": 866, "freqStart": 865, "freqEnd": 867, "dutyCycle": 100, "spacing": 0, "powerLimit": 30},</v>
       </c>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="28"/>
-      <c r="M30" s="28"/>
-      <c r="N30" s="28"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
     </row>
     <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
@@ -8885,15 +8898,15 @@
       <c r="H31" s="4">
         <v>0</v>
       </c>
-      <c r="I31" s="28" t="str">
+      <c r="I31" s="29" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "NZ865", "freqCenter": 866, "freqStart": 864, "freqEnd": 868, "dutyCycle": 100, "spacing": 0, "powerLimit": 0},</v>
       </c>
-      <c r="J31" s="28"/>
-      <c r="K31" s="28"/>
-      <c r="L31" s="28"/>
-      <c r="M31" s="28"/>
-      <c r="N31" s="28"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
     </row>
     <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
@@ -8920,15 +8933,15 @@
       <c r="H32" s="4">
         <v>16</v>
       </c>
-      <c r="I32" s="28" t="str">
+      <c r="I32" s="29" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "TH", "freqCenter": 922.5, "freqStart": 920, "freqEnd": 925, "dutyCycle": 100, "spacing": 0, "powerLimit": 16},</v>
       </c>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="28"/>
-      <c r="M32" s="28"/>
-      <c r="N32" s="28"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="29"/>
     </row>
     <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
@@ -8955,18 +8968,204 @@
       <c r="H33" s="4">
         <v>30</v>
       </c>
-      <c r="I33" s="28" t="str">
+      <c r="I33" s="29" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "Unset", "freqCenter": 915, "freqStart": 902, "freqEnd": 928, "dutyCycle": 100, "spacing": 0, "powerLimit": 30},</v>
       </c>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="28"/>
-      <c r="N33" s="28"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="29"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B37" s="23">
+        <f>E21-D21</f>
+        <v>26</v>
+      </c>
+      <c r="C37" s="30">
+        <f>B37*1000</f>
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B38" s="23">
+        <f t="shared" ref="B38:B49" si="3">E22-D22</f>
+        <v>1</v>
+      </c>
+      <c r="C38" s="30">
+        <f t="shared" ref="C38:C49" si="4">B38*1000</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="31" t="s">
+        <v>162</v>
+      </c>
+      <c r="B39" s="32">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="C39" s="33">
+        <f t="shared" si="4"/>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B40" s="23">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="C40" s="30">
+        <f t="shared" si="4"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B41" s="23">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="C41" s="30">
+        <f t="shared" si="4"/>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B42" s="23">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="C42" s="30">
+        <f t="shared" si="4"/>
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B43" s="23">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="C43" s="30">
+        <f t="shared" si="4"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B44" s="23">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="C44" s="30">
+        <f t="shared" si="4"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B45" s="23">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="C45" s="30">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B46" s="23">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="C46" s="30">
+        <f t="shared" si="4"/>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B47" s="23">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="C47" s="30">
+        <f t="shared" si="4"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B48" s="23">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="C48" s="30">
+        <f t="shared" si="4"/>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B49" s="23">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="C49" s="30">
+        <f t="shared" si="4"/>
+        <v>26000</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="I25:N25"/>
+    <mergeCell ref="I20:N20"/>
+    <mergeCell ref="I21:N21"/>
+    <mergeCell ref="I22:N22"/>
+    <mergeCell ref="I23:N23"/>
+    <mergeCell ref="I24:N24"/>
     <mergeCell ref="I32:N32"/>
     <mergeCell ref="I33:N33"/>
     <mergeCell ref="I26:N26"/>
@@ -8975,12 +9174,6 @@
     <mergeCell ref="I29:N29"/>
     <mergeCell ref="I30:N30"/>
     <mergeCell ref="I31:N31"/>
-    <mergeCell ref="I25:N25"/>
-    <mergeCell ref="I20:N20"/>
-    <mergeCell ref="I21:N21"/>
-    <mergeCell ref="I22:N22"/>
-    <mergeCell ref="I23:N23"/>
-    <mergeCell ref="I24:N24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>

<commit_message>
Added editor (New message & id only) TODO: - Add validation - Add validation prompt - Incorporate editor for remaining text fields
</commit_message>
<xml_diff>
--- a/Documentation/Tasks.xlsx
+++ b/Documentation/Tasks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Armachat-circuitpython\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Armachat\Armachat-circuitpython\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD72D78-3CA0-4DBF-8729-0197B1638A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA13B15-36D3-4F84-8EDB-78C6765B832D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="4" xr2:uid="{48331F84-D6AF-4212-9807-071E67B15285}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{48331F84-D6AF-4212-9807-071E67B15285}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -783,6 +783,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -795,17 +799,61 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="2"/>
+        </left>
+        <right style="thin">
+          <color theme="2"/>
+        </right>
+        <top style="thin">
+          <color theme="2"/>
+        </top>
+        <bottom style="thin">
+          <color theme="2"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -1128,9 +1176,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{463C985E-F91F-471A-B04D-0671E5EAB4DD}">
   <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2412,6 +2460,11 @@
       <c r="D96" s="4"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A6:D96">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>OR($D6="",NOT($D6))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2435,30 +2488,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="26"/>
+      <c r="C1" s="30"/>
       <c r="D1">
         <f>COUNTA(A6:A501)</f>
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="26"/>
+      <c r="C2" s="30"/>
       <c r="D2">
         <f>D1-COUNTIF(D6:D501,TRUE)</f>
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="26"/>
+      <c r="C3" s="30"/>
       <c r="D3" s="9">
         <f>(D1-D2)/D1</f>
         <v>0.77777777777777779</v>
@@ -2931,12 +2984,12 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -3013,12 +3066,12 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -3298,28 +3351,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="32"/>
       <c r="C1" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="32" t="s">
         <v>175</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="4">
         <v>902</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="B3" s="28"/>
+      <c r="B3" s="32"/>
       <c r="C3" s="4">
         <v>928</v>
       </c>
@@ -7944,7 +7997,7 @@
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="A6:E214">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$E6&gt;$C$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7957,7 +8010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0905176-8170-4141-BFF8-73C1F588C34D}">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -8514,14 +8567,14 @@
       <c r="H20" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="I20" s="27" t="s">
+      <c r="I20" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
@@ -8548,15 +8601,15 @@
       <c r="H21" s="4">
         <v>30</v>
       </c>
-      <c r="I21" s="29" t="str">
+      <c r="I21" s="33" t="str">
         <f>"{""" &amp;$A$20 &amp; """: """ &amp; A21 &amp; """, """  &amp; $C$20 &amp; """: " &amp; C21 &amp; ", """ &amp; $D$20 &amp; """: " &amp;D21 &amp; ", """ &amp; $E$20 &amp; """: " &amp; E21 &amp; ", """ &amp; $F$20 &amp; """: " &amp; F21 &amp; ", """ &amp; $G$20 &amp; """: " &amp; G21 &amp; ", """ &amp; $H$20 &amp; """: " &amp; H21 &amp; "},"</f>
         <v>{"region": "US", "freqCenter": 915, "freqStart": 902, "freqEnd": 928, "dutyCycle": 100, "spacing": 0, "powerLimit": 30},</v>
       </c>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="29"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
@@ -8583,15 +8636,15 @@
       <c r="H22" s="4">
         <v>12</v>
       </c>
-      <c r="I22" s="29" t="str">
+      <c r="I22" s="33" t="str">
         <f t="shared" ref="I22:I33" si="2">"{""" &amp;$A$20 &amp; """: """ &amp; A22 &amp; """, """  &amp; $C$20 &amp; """: " &amp; C22 &amp; ", """ &amp; $D$20 &amp; """: " &amp;D22 &amp; ", """ &amp; $E$20 &amp; """: " &amp; E22 &amp; ", """ &amp; $F$20 &amp; """: " &amp; F22 &amp; ", """ &amp; $G$20 &amp; """: " &amp; G22 &amp; ", """ &amp; $H$20 &amp; """: " &amp; H22 &amp; "},"</f>
         <v>{"region": "EU433", "freqCenter": 433.5, "freqStart": 433, "freqEnd": 434, "dutyCycle": 10, "spacing": 0, "powerLimit": 12},</v>
       </c>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="29"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
     </row>
     <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
@@ -8618,15 +8671,15 @@
       <c r="H23" s="4">
         <v>16</v>
       </c>
-      <c r="I23" s="29" t="str">
+      <c r="I23" s="33" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "EU868", "freqCenter": 869.525, "freqStart": 869.4, "freqEnd": 869.65, "dutyCycle": 10, "spacing": 0, "powerLimit": 16},</v>
       </c>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="29"/>
-      <c r="N23" s="29"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
     </row>
     <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -8653,15 +8706,15 @@
       <c r="H24" s="4">
         <v>19</v>
       </c>
-      <c r="I24" s="29" t="str">
+      <c r="I24" s="33" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "CN", "freqCenter": 490, "freqStart": 470, "freqEnd": 510, "dutyCycle": 100, "spacing": 0, "powerLimit": 19},</v>
       </c>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="29"/>
-      <c r="N24" s="29"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
     </row>
     <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -8688,15 +8741,15 @@
       <c r="H25" s="4">
         <v>16</v>
       </c>
-      <c r="I25" s="29" t="str">
+      <c r="I25" s="33" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "JP", "freqCenter": 924.3, "freqStart": 920.8, "freqEnd": 927.8, "dutyCycle": 100, "spacing": 0, "powerLimit": 16},</v>
       </c>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
-      <c r="N25" s="29"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
     </row>
     <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -8723,15 +8776,15 @@
       <c r="H26" s="4">
         <v>30</v>
       </c>
-      <c r="I26" s="29" t="str">
+      <c r="I26" s="33" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "ANZ", "freqCenter": 921.5, "freqStart": 915, "freqEnd": 928, "dutyCycle": 100, "spacing": 0, "powerLimit": 30},</v>
       </c>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
-      <c r="N26" s="29"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
     </row>
     <row r="27" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -8758,15 +8811,15 @@
       <c r="H27" s="4">
         <v>20</v>
       </c>
-      <c r="I27" s="29" t="str">
+      <c r="I27" s="33" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "RU", "freqCenter": 868.95, "freqStart": 868.7, "freqEnd": 869.2, "dutyCycle": 100, "spacing": 0, "powerLimit": 20},</v>
       </c>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="29"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
     </row>
     <row r="28" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
@@ -8793,15 +8846,15 @@
       <c r="H28" s="4">
         <v>0</v>
       </c>
-      <c r="I28" s="29" t="str">
+      <c r="I28" s="33" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "KR", "freqCenter": 921.5, "freqStart": 920, "freqEnd": 923, "dutyCycle": 100, "spacing": 0, "powerLimit": 0},</v>
       </c>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
     </row>
     <row r="29" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
@@ -8828,15 +8881,15 @@
       <c r="H29" s="4">
         <v>0</v>
       </c>
-      <c r="I29" s="29" t="str">
+      <c r="I29" s="33" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "TW", "freqCenter": 922.5, "freqStart": 920, "freqEnd": 925, "dutyCycle": 100, "spacing": 0, "powerLimit": 0},</v>
       </c>
-      <c r="J29" s="29"/>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="29"/>
-      <c r="N29" s="29"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
     </row>
     <row r="30" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
@@ -8863,15 +8916,15 @@
       <c r="H30" s="4">
         <v>30</v>
       </c>
-      <c r="I30" s="29" t="str">
+      <c r="I30" s="33" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "IN", "freqCenter": 866, "freqStart": 865, "freqEnd": 867, "dutyCycle": 100, "spacing": 0, "powerLimit": 30},</v>
       </c>
-      <c r="J30" s="29"/>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="29"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="33"/>
     </row>
     <row r="31" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
@@ -8898,15 +8951,15 @@
       <c r="H31" s="4">
         <v>0</v>
       </c>
-      <c r="I31" s="29" t="str">
+      <c r="I31" s="33" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "NZ865", "freqCenter": 866, "freqStart": 864, "freqEnd": 868, "dutyCycle": 100, "spacing": 0, "powerLimit": 0},</v>
       </c>
-      <c r="J31" s="29"/>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="29"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="33"/>
+      <c r="N31" s="33"/>
     </row>
     <row r="32" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
@@ -8933,15 +8986,15 @@
       <c r="H32" s="4">
         <v>16</v>
       </c>
-      <c r="I32" s="29" t="str">
+      <c r="I32" s="33" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "TH", "freqCenter": 922.5, "freqStart": 920, "freqEnd": 925, "dutyCycle": 100, "spacing": 0, "powerLimit": 16},</v>
       </c>
-      <c r="J32" s="29"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="33"/>
     </row>
     <row r="33" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
@@ -8968,15 +9021,15 @@
       <c r="H33" s="4">
         <v>30</v>
       </c>
-      <c r="I33" s="29" t="str">
+      <c r="I33" s="33" t="str">
         <f t="shared" si="2"/>
         <v>{"region": "Unset", "freqCenter": 915, "freqStart": 902, "freqEnd": 928, "dutyCycle": 100, "spacing": 0, "powerLimit": 30},</v>
       </c>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
-      <c r="N33" s="29"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="33"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
@@ -8997,7 +9050,7 @@
         <f>E21-D21</f>
         <v>26</v>
       </c>
-      <c r="C37" s="30">
+      <c r="C37" s="26">
         <f>B37*1000</f>
         <v>26000</v>
       </c>
@@ -9010,20 +9063,20 @@
         <f t="shared" ref="B38:B49" si="3">E22-D22</f>
         <v>1</v>
       </c>
-      <c r="C38" s="30">
+      <c r="C38" s="26">
         <f t="shared" ref="C38:C49" si="4">B38*1000</f>
         <v>1000</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="27" t="s">
         <v>162</v>
       </c>
-      <c r="B39" s="32">
+      <c r="B39" s="28">
         <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
-      <c r="C39" s="33">
+      <c r="C39" s="29">
         <f t="shared" si="4"/>
         <v>250</v>
       </c>
@@ -9036,7 +9089,7 @@
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="C40" s="30">
+      <c r="C40" s="26">
         <f t="shared" si="4"/>
         <v>40000</v>
       </c>
@@ -9049,7 +9102,7 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="C41" s="30">
+      <c r="C41" s="26">
         <f t="shared" si="4"/>
         <v>7000</v>
       </c>
@@ -9062,7 +9115,7 @@
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="C42" s="30">
+      <c r="C42" s="26">
         <f t="shared" si="4"/>
         <v>13000</v>
       </c>
@@ -9075,7 +9128,7 @@
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
-      <c r="C43" s="30">
+      <c r="C43" s="26">
         <f t="shared" si="4"/>
         <v>500</v>
       </c>
@@ -9088,7 +9141,7 @@
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="C44" s="30">
+      <c r="C44" s="26">
         <f t="shared" si="4"/>
         <v>3000</v>
       </c>
@@ -9101,7 +9154,7 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="C45" s="30">
+      <c r="C45" s="26">
         <f t="shared" si="4"/>
         <v>5000</v>
       </c>
@@ -9114,7 +9167,7 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="C46" s="30">
+      <c r="C46" s="26">
         <f t="shared" si="4"/>
         <v>2000</v>
       </c>
@@ -9127,7 +9180,7 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="C47" s="30">
+      <c r="C47" s="26">
         <f t="shared" si="4"/>
         <v>4000</v>
       </c>
@@ -9140,7 +9193,7 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="C48" s="30">
+      <c r="C48" s="26">
         <f t="shared" si="4"/>
         <v>5000</v>
       </c>
@@ -9153,19 +9206,13 @@
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="C49" s="30">
+      <c r="C49" s="26">
         <f t="shared" si="4"/>
         <v>26000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="I25:N25"/>
-    <mergeCell ref="I20:N20"/>
-    <mergeCell ref="I21:N21"/>
-    <mergeCell ref="I22:N22"/>
-    <mergeCell ref="I23:N23"/>
-    <mergeCell ref="I24:N24"/>
     <mergeCell ref="I32:N32"/>
     <mergeCell ref="I33:N33"/>
     <mergeCell ref="I26:N26"/>
@@ -9174,6 +9221,12 @@
     <mergeCell ref="I29:N29"/>
     <mergeCell ref="I30:N30"/>
     <mergeCell ref="I31:N31"/>
+    <mergeCell ref="I25:N25"/>
+    <mergeCell ref="I20:N20"/>
+    <mergeCell ref="I21:N21"/>
+    <mergeCell ref="I22:N22"/>
+    <mergeCell ref="I23:N23"/>
+    <mergeCell ref="I24:N24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>

<commit_message>
Added validation to editor
</commit_message>
<xml_diff>
--- a/Documentation/Tasks.xlsx
+++ b/Documentation/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Armachat\Armachat-circuitpython\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA13B15-36D3-4F84-8EDB-78C6765B832D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54F2146-A77F-43B6-888C-A736428BE749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{48331F84-D6AF-4212-9807-071E67B15285}"/>
   </bookViews>
@@ -805,7 +805,17 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -829,40 +839,6 @@
           <color theme="2"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1177,8 +1153,8 @@
   <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,7 +1179,7 @@
       </c>
       <c r="D2">
         <f>D1-COUNTIF(D6:D502,TRUE)</f>
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1212,7 +1188,7 @@
       </c>
       <c r="D3" s="9">
         <f>(D1-D2)/D1</f>
-        <v>0.75824175824175821</v>
+        <v>0.76923076923076927</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2053,7 +2029,9 @@
       <c r="C66" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D66" s="4"/>
+      <c r="D66" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
@@ -2461,7 +2439,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6:D96">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>OR($D6="",NOT($D6))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7997,7 +7975,7 @@
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="A6:E214">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$E6&gt;$C$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9213,6 +9191,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="I25:N25"/>
+    <mergeCell ref="I20:N20"/>
+    <mergeCell ref="I21:N21"/>
+    <mergeCell ref="I22:N22"/>
+    <mergeCell ref="I23:N23"/>
+    <mergeCell ref="I24:N24"/>
     <mergeCell ref="I32:N32"/>
     <mergeCell ref="I33:N33"/>
     <mergeCell ref="I26:N26"/>
@@ -9221,12 +9205,6 @@
     <mergeCell ref="I29:N29"/>
     <mergeCell ref="I30:N30"/>
     <mergeCell ref="I31:N31"/>
-    <mergeCell ref="I25:N25"/>
-    <mergeCell ref="I20:N20"/>
-    <mergeCell ref="I21:N21"/>
-    <mergeCell ref="I22:N22"/>
-    <mergeCell ref="I23:N23"/>
-    <mergeCell ref="I24:N24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>

<commit_message>
Added radio code Working - Receiving Messages - Sending Message (Assumed as not received on other Armachat)
To Do
- Display messages
- Send confirmation on receipt
- Update status when receiving confirmation
</commit_message>
<xml_diff>
--- a/Documentation/Tasks.xlsx
+++ b/Documentation/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Armachat\Armachat-circuitpython\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54F2146-A77F-43B6-888C-A736428BE749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2B5859-1024-4DEA-8EEC-D12D6FE0F43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{48331F84-D6AF-4212-9807-071E67B15285}"/>
   </bookViews>
@@ -1153,8 +1153,8 @@
   <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D67" sqref="D67"/>
+      <pane ySplit="5" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="D2">
         <f>D1-COUNTIF(D6:D502,TRUE)</f>
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1188,7 +1188,7 @@
       </c>
       <c r="D3" s="9">
         <f>(D1-D2)/D1</f>
-        <v>0.76923076923076927</v>
+        <v>0.81318681318681318</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1327,7 +1327,9 @@
       <c r="C14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="4"/>
+      <c r="D14" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -2411,7 +2413,9 @@
       <c r="C94" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D94" s="4"/>
+      <c r="D94" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
@@ -2423,7 +2427,9 @@
       <c r="C95" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="D95" s="4"/>
+      <c r="D95" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
@@ -2435,7 +2441,9 @@
       <c r="C96" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="D96" s="4"/>
+      <c r="D96" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6:D96">
@@ -9191,12 +9199,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="I25:N25"/>
-    <mergeCell ref="I20:N20"/>
-    <mergeCell ref="I21:N21"/>
-    <mergeCell ref="I22:N22"/>
-    <mergeCell ref="I23:N23"/>
-    <mergeCell ref="I24:N24"/>
     <mergeCell ref="I32:N32"/>
     <mergeCell ref="I33:N33"/>
     <mergeCell ref="I26:N26"/>
@@ -9205,6 +9207,12 @@
     <mergeCell ref="I29:N29"/>
     <mergeCell ref="I30:N30"/>
     <mergeCell ref="I31:N31"/>
+    <mergeCell ref="I25:N25"/>
+    <mergeCell ref="I20:N20"/>
+    <mergeCell ref="I21:N21"/>
+    <mergeCell ref="I22:N22"/>
+    <mergeCell ref="I23:N23"/>
+    <mergeCell ref="I24:N24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>

<commit_message>
All seems to be working fine on Armachat Compact TODO: Test and fix for Amrachat Watch
</commit_message>
<xml_diff>
--- a/Documentation/Tasks.xlsx
+++ b/Documentation/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Armachat\Armachat-circuitpython\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2B5859-1024-4DEA-8EEC-D12D6FE0F43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A863127-C879-4F3C-8427-0E58956D3740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{48331F84-D6AF-4212-9807-071E67B15285}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="192">
   <si>
     <t>Screen</t>
   </si>
@@ -613,6 +613,9 @@
   </si>
   <si>
     <t>bw (MHz)</t>
+  </si>
+  <si>
+    <t>B-Long</t>
   </si>
 </sst>
 </file>
@@ -1153,8 +1156,8 @@
   <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D97" sqref="D97"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,7 +1182,7 @@
       </c>
       <c r="D2">
         <f>D1-COUNTIF(D6:D502,TRUE)</f>
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1188,7 +1191,7 @@
       </c>
       <c r="D3" s="9">
         <f>(D1-D2)/D1</f>
-        <v>0.81318681318681318</v>
+        <v>0.93406593406593408</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1341,7 +1344,9 @@
       <c r="C15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -1393,7 +1398,9 @@
       <c r="C19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="4"/>
+      <c r="D19" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
@@ -1405,31 +1412,37 @@
       <c r="C20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="4"/>
+      <c r="D20" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="4"/>
+      <c r="D21" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>6</v>
+        <v>191</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="4"/>
+      <c r="D22" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
@@ -1441,7 +1454,9 @@
       <c r="C23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="4"/>
+      <c r="D23" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
@@ -1453,7 +1468,9 @@
       <c r="C24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="4"/>
+      <c r="D24" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -1465,7 +1482,9 @@
       <c r="C25" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="4"/>
+      <c r="D25" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
@@ -1477,7 +1496,9 @@
       <c r="C26" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D26" s="4"/>
+      <c r="D26" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
@@ -1489,7 +1510,9 @@
       <c r="C27" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="4"/>
+      <c r="D27" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
@@ -1501,7 +1524,9 @@
       <c r="C28" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="4"/>
+      <c r="D28" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
@@ -9199,6 +9224,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="I25:N25"/>
+    <mergeCell ref="I20:N20"/>
+    <mergeCell ref="I21:N21"/>
+    <mergeCell ref="I22:N22"/>
+    <mergeCell ref="I23:N23"/>
+    <mergeCell ref="I24:N24"/>
     <mergeCell ref="I32:N32"/>
     <mergeCell ref="I33:N33"/>
     <mergeCell ref="I26:N26"/>
@@ -9207,12 +9238,6 @@
     <mergeCell ref="I29:N29"/>
     <mergeCell ref="I30:N30"/>
     <mergeCell ref="I31:N31"/>
-    <mergeCell ref="I25:N25"/>
-    <mergeCell ref="I20:N20"/>
-    <mergeCell ref="I21:N21"/>
-    <mergeCell ref="I22:N22"/>
-    <mergeCell ref="I23:N23"/>
-    <mergeCell ref="I24:N24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>